<commit_message>
Added more useful features. Got up to Union types
</commit_message>
<xml_diff>
--- a/JavaScript and TypeScript Cheatsheet.xlsx
+++ b/JavaScript and TypeScript Cheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739A1B7B-0403-4D96-8C83-AEB5E8E33916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DB367E-FD4F-40D9-9930-6EF4CB8CA73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="-765" windowWidth="14610" windowHeight="15585" firstSheet="2" activeTab="2" xr2:uid="{8E0EA162-069A-4055-969A-D163D2934874}"/>
+    <workbookView xWindow="-28920" yWindow="-885" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{8E0EA162-069A-4055-969A-D163D2934874}"/>
   </bookViews>
   <sheets>
     <sheet name="JavaScript Basics" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
   <si>
     <t>Concept</t>
   </si>
@@ -144,9 +144,6 @@
 let name1 = user.name</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>How to install TypeScript</t>
   </si>
   <si>
@@ -264,6 +261,390 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>let myName: string = "conor";
+let myAge: number = "27;
+let isActive: boolean = true;
+let myArray: number[] = [1, 2, 3, 4, 5];
+let myArray2: string[] = ["yeah", "no", "maybe"]
+let myObject: object = {name: "conor", age: "27}</t>
+  </si>
+  <si>
+    <t>Specify the type of a varaible when we create it</t>
+  </si>
+  <si>
+    <t>When we create a variable in TypeScript, we have the optional (but highly-recommended) option of specifying the type of the variable that we're creating. This makes TypeScript code much more familiar to a language such as Java, where you have to specify the type of the variable that you're creating.</t>
+  </si>
+  <si>
+    <t>Specify the type as you're passing it into the function, as well as when returning a value from a function</t>
+  </si>
+  <si>
+    <t>When we pass through a variable into a function, we need to be able to specify the type of the variable that we're passing through.
+In addition, we can specify what kind of returns we'd like by adding return type annotations.</t>
+  </si>
+  <si>
+    <t>Specifying complex types into functions</t>
+  </si>
+  <si>
+    <t>function printCoord(pt: { x: number; y: number }) {
+  console.log("The coordinate's x value is " + pt.x);
+  console.log("The coordinate's y value is " + pt.y);
+}
+printCoord({ x: 3, y: 7 });
+function printName(obj: { first: string; last?: string }) {
+  console.log(obj)
+}
+// Both OK
+printName({ first: "Bob" });
+printName({ first: "Alice", last: "Alisson" });</t>
+  </si>
+  <si>
+    <t>The any type</t>
+  </si>
+  <si>
+    <t>In JavaScript, a variable is assumed to have the "any" type. This means that it can be of any type whatsoever: string, number, boolean, etc. Although this can be good in certain places, overall, with respect to safety, it's always better to force the type such as in TypeScript.</t>
+  </si>
+  <si>
+    <t>function greet (name: string, age: number) {…}
+function addNumber(num: number): number {return num + 2;}</t>
+  </si>
+  <si>
+    <t>Normal functions</t>
+  </si>
+  <si>
+    <t>Ordinary functions are written like this</t>
+  </si>
+  <si>
+    <t>More efficient way of writing function</t>
+  </si>
+  <si>
+    <t>let addThree = (num) =&gt;{
+  return num + 3;
+}</t>
+  </si>
+  <si>
+    <t>function addTwo(num) {
+  return num + 2;
+}</t>
+  </si>
+  <si>
+    <t>Return multiple values in a fuctions</t>
+  </si>
+  <si>
+    <t>let returnTwoStrings = () =&gt; {
+  return ["string1", "string2"]
+}
+let [str1, str2] = getTwoStrings();</t>
+  </si>
+  <si>
+    <t>Returning multiple values, while specifying the return types</t>
+  </si>
+  <si>
+    <t>function getTwoStrings(): [string, string] {
+    return ["string1", "string2"];
+}</t>
+  </si>
+  <si>
+    <t>In the first one, we are passing through a key-value pair, which we are calling pt. Therefore to grab x, or y, we simple do pt.x, pt.y, and for each of the values we are specifying the type of each of the values within the coordinate.
+For the second example, we are doing the same thing, but we are saying last?: string. This means that the second variable is optional. If there is a last value, then we are specifying that this is a string. If not, then the code won't fail. If we aren't returning anything, then we should force it to return void</t>
+  </si>
+  <si>
+    <t>Specifying return values</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We can specify the type of the value that we want to return by using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: type </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">after our bracket. If we aren't returning any values, then we can ensure this by using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: void</t>
+    </r>
+  </si>
+  <si>
+    <t>Forcing a function to never return a value</t>
+  </si>
+  <si>
+    <t>function handleError(errorMessage: string): never {
+    throw new Error(errorMessage);
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We can use the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>never</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> type for this code to make sure that we never return a value. It looks very similar to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>void</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, but actually this is usually used when we need to throw an error message using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>throw new Error(etc)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, instead of console.log();</t>
+    </r>
+  </si>
+  <si>
+    <t>function getString(): string {
+    return "string1";
+}
+function createCourse(): {name: string, price: number} {
+  return {name: "course", price: 100};}</t>
+  </si>
+  <si>
+    <t>Creating type aliases</t>
+  </si>
+  <si>
+    <t>type User = {
+    name: string;
+    email: string;
+    isActive: boolean;
+    age: number;
+};
+const newUser: User = { name: 'Alice', email: 'alice@example.com', isActive: true, age: 25 };
+function showUser(user: User) {
+    console.log(user.name); console.log(user.email);
+    console.log(user.isActive); console.log(user.age);
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Can be very useful, especially for more complex data types such as objects. We can define the type, in this example, type user, and then create new User elements through const newUser: User = {…}.
+Defining the User type also means that when we pass through the variable to a function, instead of passing through each of the specific types, we can simply pass through a User type. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">user: User. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Just like in Java where you can specify the object type, here we can have the object time also.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Very useful overall in the long run.</t>
+    </r>
+  </si>
+  <si>
+    <t>Using readonly to create variables that don't change their values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type User = {
+    readonly name: string;
+    readonly email: string;
+    isActive: boolean;
+    age: number;
+};
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Using readonly in TypeScript is slightly unusual. In some ways, it's very similar to the const keyword for creating values that don't change, so in theory, you could have some code like: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>let numbers: readonly number[] = [1, 2, 3];</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> However readonly is really more used for individual fields within a key-value pair, or perhaps within a class. You might want some of the fields to never change, and others to change. For example, the name and email of a user can't change, but their age and isActive status can change. In this instance, you put readonly in front of name and email, and not in front of isActive and age.</t>
+    </r>
+  </si>
+  <si>
+    <t>type User = {
+    readonly name: string,
+    age: number,
+    creditCardDetails?: number,
+};
+let user: User = {name: 'John', age: 30, creditCardDetails = 123123};
+user.name = 'Jane';
+user.age = 40;
+user.creditCardDetails = 1234567890</t>
+  </si>
+  <si>
+    <t>Optional variables within a key-value object or function</t>
+  </si>
+  <si>
+    <t>TypeScript much more easily allows us to have optional values that are not absolutely required to be passed, or not passed through to a function or a key-value pair. To highlight that this is the situation, we can put a question mark at the end of the optional variable.
+A function works in a similar way, and we can do it like this:
+function getDetails(name: string, age: number, email?: string) {...}</t>
+  </si>
+  <si>
+    <t>The example below may look like a more convoluted method of writing code, but the reality is that it's an even more useful way of enforcing the type, and of separating the various bits. We can change the structure of card-related information by just changing the types of previous variables up top.
+type cardNumber = {cardNumber: string,}
+type cardDate = {cardDate: string,}
+type cardDetails = cardNumber &amp; cardDate &amp; {cvv: number,};
+let card1: cardDetails = {
+    cardNumber: '1234567890',
+    cardDate: '12/2023',
+    cvv: 123
+}</t>
+  </si>
+  <si>
+    <t>With number[] and string[], we are also able to define an object type array (e.g. a list of User objects could be const users: User[] = [].
+Example code:
+const users: User[] = []
+users.push({ name: 'John', age: 30 })
+users.push({ name: 'Jane', age: 25 })</t>
+  </si>
+  <si>
+    <t>Forcing type for multi-dimensional array</t>
+  </si>
+  <si>
+    <t>const MLModel: number[][] = [
+  [255, 255, 255],
+  [],
+]</t>
+  </si>
+  <si>
+    <t>Union type</t>
+  </si>
+  <si>
+    <t>let id: number | string = 33;
+id = "43";
+type User = {
+  name: string;
+  id: string | number;
+}</t>
+  </si>
+  <si>
+    <t>Possibly one of the most useful aspects of TypeScript, union means that when you receive a variable, it can be of more than just one type. A variable being sent to a function can be a string or a number, or an array, of any other specified type, and it's all fine. We can use union types anywhere in TS, whether it be for a primative data type, a function, or an object.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can have union types referring to separate </t>
   </si>
 </sst>
 </file>
@@ -316,7 +697,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -407,16 +788,112 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -429,27 +906,135 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+  <dxfs count="25">
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -475,18 +1060,185 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -497,152 +1249,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -683,41 +1289,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D67A83B5-6DB9-4D1D-B1E1-F7D382D58B3C}" name="Table1" displayName="Table1" ref="A1:E8" totalsRowShown="0">
-  <autoFilter ref="A1:E8" xr:uid="{D67A83B5-6DB9-4D1D-B1E1-F7D382D58B3C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D67A83B5-6DB9-4D1D-B1E1-F7D382D58B3C}" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:E11" xr:uid="{D67A83B5-6DB9-4D1D-B1E1-F7D382D58B3C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{090BD192-1D20-47D2-8F6F-5AF92E218BEB}" name="Concept" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{25DDA5F8-4AB0-4AAC-ABCA-BF59415478C2}" name="Code" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{C1DAB56A-CB82-4D25-8492-48FBFC047ECF}" name="Explained" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{D17684CE-80C0-4E1E-AA09-5D5E6B7F0C8E}" name="Notes" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{AD919A87-3529-4F1F-B0E4-2D6B1AE0970D}" name="Images" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{090BD192-1D20-47D2-8F6F-5AF92E218BEB}" name="Concept" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{25DDA5F8-4AB0-4AAC-ABCA-BF59415478C2}" name="Code" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{C1DAB56A-CB82-4D25-8492-48FBFC047ECF}" name="Explained" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{D17684CE-80C0-4E1E-AA09-5D5E6B7F0C8E}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{AD919A87-3529-4F1F-B0E4-2D6B1AE0970D}" name="Images" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86A51DF5-045C-430C-8E6C-5414FCA48178}" name="Table2" displayName="Table2" ref="A1:D4" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86A51DF5-045C-430C-8E6C-5414FCA48178}" name="Table2" displayName="Table2" ref="A1:D4" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21">
   <autoFilter ref="A1:D4" xr:uid="{86A51DF5-045C-430C-8E6C-5414FCA48178}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{909A7DFE-AF7A-4AEE-B64B-4DFD1577B15C}" name="Concept" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{8C0E44D8-D479-472D-9150-29C9A92B5D3C}" name="Explained" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{1BF832DC-50E8-42B0-98A6-D7D3C3D87754}" name="Notes" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{F8C9EC3F-25A2-4D4C-90B0-3BF5E194A063}" name="Images" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{909A7DFE-AF7A-4AEE-B64B-4DFD1577B15C}" name="Concept" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{8C0E44D8-D479-472D-9150-29C9A92B5D3C}" name="Explained" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{1BF832DC-50E8-42B0-98A6-D7D3C3D87754}" name="Notes" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{F8C9EC3F-25A2-4D4C-90B0-3BF5E194A063}" name="Images" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}" name="Table3" displayName="Table3" ref="A1:E2" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
-  <autoFilter ref="A1:E2" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}" name="Table3" displayName="Table3" ref="A1:E12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:E12" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3A580996-E5D3-4561-AC07-BA4822C0708C}" name="Concept" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{DA354905-1BC8-460D-98B4-ADED2D10AFBF}" name="Code" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{C6C4CC59-F9BA-49FA-8B0F-D7372B8894D2}" name="Explained" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{936E524D-0762-4E82-A3EF-588C1391A681}" name="Notes" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{400184B0-77C8-40AE-9D2A-88E525B9230C}" name="Images" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3A580996-E5D3-4561-AC07-BA4822C0708C}" name="Concept" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{DA354905-1BC8-460D-98B4-ADED2D10AFBF}" name="Code" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{C6C4CC59-F9BA-49FA-8B0F-D7372B8894D2}" name="Explained" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{936E524D-0762-4E82-A3EF-588C1391A681}" name="Notes" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{400184B0-77C8-40AE-9D2A-88E525B9230C}" name="Images" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1020,48 +1626,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1248A541-ED2E-47A6-9221-52FC18FFA65E}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="49.28515625" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="65.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="47.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1076,7 +1683,7 @@
       <c r="D3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="13"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1089,7 +1696,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="13"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -1102,18 +1709,18 @@
         <v>28</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="13"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -1124,14 +1731,53 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1176,31 +1822,31 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="4"/>
     </row>
   </sheetData>
@@ -1212,7 +1858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FF2D82-85A9-4218-B047-8A72B9F1F6B9}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1252,18 +1898,18 @@
     </row>
     <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1276,43 +1922,183 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E945EC2-D845-46A8-A317-7E66B9F1414A}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="49.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="56" style="8" customWidth="1"/>
     <col min="3" max="3" width="62.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="83.140625" style="8" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" style="8" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>31</v>
-      </c>
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+    </row>
+    <row r="12" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated JS and TS cheatsheet
</commit_message>
<xml_diff>
--- a/JavaScript and TypeScript Cheatsheet.xlsx
+++ b/JavaScript and TypeScript Cheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C402E34C-D351-4D7F-BB81-E13CF8F3C200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836E283E-6E25-4D8E-831C-F96021567126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="18960" windowHeight="17385" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{8E0EA162-069A-4055-969A-D163D2934874}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" tabRatio="650" activeTab="1" xr2:uid="{8E0EA162-069A-4055-969A-D163D2934874}"/>
   </bookViews>
   <sheets>
     <sheet name="JavaScript Basics" sheetId="1" r:id="rId1"/>
@@ -2164,7 +2164,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2326,8 +2326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A27C8EB-46AB-40DE-A121-941C9B944C1E}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2467,7 +2467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E945EC2-D845-46A8-A317-7E66B9F1414A}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Completed the TypeScript portion for now
I've filled in all the TypeScript portions of it. I now want to try and use it somewhere. I'm still not that good at Web Dev, but if I can improve it, that would be great. Want to learn a little bit of Bulma CSS Framework (very simple, but effective framework), then make something
</commit_message>
<xml_diff>
--- a/JavaScript and TypeScript Cheatsheet.xlsx
+++ b/JavaScript and TypeScript Cheatsheet.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836E283E-6E25-4D8E-831C-F96021567126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FCF58F-05A4-42B5-964D-62CE1163719F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" tabRatio="650" activeTab="1" xr2:uid="{8E0EA162-069A-4055-969A-D163D2934874}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" tabRatio="717" activeTab="3" xr2:uid="{8E0EA162-069A-4055-969A-D163D2934874}"/>
   </bookViews>
   <sheets>
     <sheet name="JavaScript Basics" sheetId="1" r:id="rId1"/>
     <sheet name="JavaScript Intermediate" sheetId="2" r:id="rId2"/>
     <sheet name="TypeScript Explained" sheetId="3" r:id="rId3"/>
-    <sheet name="TypeScript Basics" sheetId="4" r:id="rId4"/>
+    <sheet name="All of TypeScript" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="125">
   <si>
     <t>Concept</t>
   </si>
@@ -1133,9 +1133,6 @@
 }</t>
   </si>
   <si>
-    <t>TypeScript allows us to specify whether or not the attributes in a field are public or private. Therefore in order to grab the data, or change the data, we need to create getters and setters</t>
-  </si>
-  <si>
     <t>An alternative way of creating a class with public and private attributes, but with fewer lines of syntax is to write it like this:
 class Student {
     constructor(private name: string, public age: number) {
@@ -1179,14 +1176,149 @@
 }</t>
   </si>
   <si>
-    <t>Protected is not really used that much, but it basically refers to fields of a class which can be accessed exclusively within its own class, as well as within subclasses.</t>
+    <t>TypeScript allows us to specify whether or not the attributes in a field are public or private. Therefore in order to grab the data, or change the data, we need to create getters and setters. We can also determine whether a method is private or public</t>
+  </si>
+  <si>
+    <t>Protected is not really used that much, but it basically refers to fields of a class which can be accessed exclusively within its own class, as well as within subclasses. Exclusively used within the super class and sub class. Again, very rare to use</t>
+  </si>
+  <si>
+    <t>Abstract classes</t>
+  </si>
+  <si>
+    <t>abstract class TakePhoto {
+    constructor(
+        public cameraMode: "portrait" | "landscape",
+        public filter: string,
+    ) {
+    }
+}
+class Instagram extends TakePhoto {
+}
+const conorInstagramPhoto = new Instagram("portrait", "black and white");</t>
+  </si>
+  <si>
+    <t>Abstract classes are really rarely ever used, because any class that is abstract you're not able to create one of it directly. It's like the blueprint class which is then used as an extension for other classes.
+A final thing to mention: you can also have abstract methods for your class. But if this is the case, they it means that you must implement the method in one of the subclasses.</t>
+  </si>
+  <si>
+    <t>abstract class TakePhoto {
+    constructor(...) { }
+    abstract getSapia(): void;
+    getReelTime(): number {
+        return 9;
+    }
+}
+class Instagram extends TakePhoto {
+    constructor(...) {
+    getSapia() {
+        console.log("Getting Sapia");
+    }
+}</t>
+  </si>
+  <si>
+    <t>Generics</t>
+  </si>
+  <si>
+    <t>function identity&lt;T&gt;(arg: T): T {
+    return arg;
+}
+identity("yeah");</t>
+  </si>
+  <si>
+    <t>We can force the type of the entire function through this method. This means that the function is able to accept any type of variable, but whatever variable is selected, must be the returned type. So it's almost the same as any, as it takes any, but it then forces everything else to be of the same type as what was passed through.</t>
+  </si>
+  <si>
+    <t>We can actually have as many of these values as we'd like:
+function func1&lt;T, U, V&gt;(value1: T… etc)</t>
+  </si>
+  <si>
+    <t>In operator narrowing</t>
+  </si>
+  <si>
+    <t>interface Admin {
+    name: string,
+    email: string,
+    isAdmin: boolean
+}
+interface User {
+    name: string,
+    email: string
+}
+function redirect(Account: Admin | User) {
+    if ('isAdmin' in Account) {
+        console.log('Redirecting to admin dashboard');
+    } else {
+        console.log('Redirecting to user dashboard');
+    }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A slightly unusual feature within TypeScript, we are able to select a specific field within an interface by using the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operator. In a similar way we can check whether an item is within a list in Python using in, we can check the interface keys using this feature, helping us to distinguish easily between two features.</t>
+    </r>
+  </si>
+  <si>
+    <t>The instanceOf operator</t>
+  </si>
+  <si>
+    <t>interface Date {
+    day: number,
+    month: number,
+    year: number
+}
+function checkDate(x: Date | number) {
+    if (x instanceof Date) {
+        console.log('This is a Date alright');
+    } else {
+        console.log('This is not a Date');
+    }
+}</t>
+  </si>
+  <si>
+    <t>The instanceOf operator is used to determine whether or not the object being compared is an instance of a specific interface/class.</t>
+  </si>
+  <si>
+    <t>Export</t>
+  </si>
+  <si>
+    <t>export {fun1, type1, interface1};
+Alternative method:
+export const foo: string = "foo"
+export function bar(): void {
+  console.log("bar")
+}</t>
+  </si>
+  <si>
+    <t>Allows you to use modules, compounds, etc in other program files.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1851,8 +1983,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}" name="Table3" displayName="Table3" ref="A1:E20" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:E20" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}" name="Table3" displayName="Table3" ref="A1:E25" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E25" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3A580996-E5D3-4561-AC07-BA4822C0708C}" name="Concept" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{DA354905-1BC8-460D-98B4-ADED2D10AFBF}" name="Code" dataDxfId="3"/>
@@ -2164,10 +2296,10 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="8" customWidth="1"/>
     <col min="2" max="2" width="49.28515625" style="8" customWidth="1"/>
@@ -2177,7 +2309,7 @@
     <col min="6" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2194,7 +2326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
@@ -2205,7 +2337,7 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2220,7 +2352,7 @@
       </c>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
@@ -2233,7 +2365,7 @@
       <c r="D4" s="10"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="60">
       <c r="A5" s="10" t="s">
         <v>26</v>
       </c>
@@ -2246,7 +2378,7 @@
       <c r="D5" s="10"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="12" t="s">
         <v>29</v>
       </c>
@@ -2257,7 +2389,7 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="10" t="s">
         <v>24</v>
       </c>
@@ -2268,7 +2400,7 @@
       <c r="D7" s="10"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="60">
       <c r="A8" s="12" t="s">
         <v>42</v>
       </c>
@@ -2279,7 +2411,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="45">
       <c r="A9" s="17" t="s">
         <v>45</v>
       </c>
@@ -2292,7 +2424,7 @@
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45">
       <c r="A10" s="17" t="s">
         <v>47</v>
       </c>
@@ -2303,7 +2435,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="60">
       <c r="A11" s="17" t="s">
         <v>50</v>
       </c>
@@ -2326,11 +2458,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A27C8EB-46AB-40DE-A121-941C9B944C1E}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
     <col min="2" max="2" width="49.28515625" customWidth="1"/>
@@ -2339,7 +2471,7 @@
     <col min="5" max="5" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2356,7 +2488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="120">
       <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
@@ -2371,7 +2503,7 @@
       </c>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="75">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -2397,7 +2529,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="8" customWidth="1"/>
     <col min="2" max="2" width="119" style="8" customWidth="1"/>
@@ -2406,7 +2538,7 @@
     <col min="5" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2420,7 +2552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="90">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -2431,7 +2563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="60">
       <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
@@ -2439,7 +2571,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" s="8" t="s">
         <v>33</v>
       </c>
@@ -2447,7 +2579,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="195">
       <c r="A5" s="8" t="s">
         <v>93</v>
       </c>
@@ -2465,13 +2597,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E945EC2-D845-46A8-A317-7E66B9F1414A}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="8" customWidth="1"/>
     <col min="2" max="2" width="56" style="8" customWidth="1"/>
@@ -2481,7 +2613,7 @@
     <col min="6" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2498,7 +2630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="90">
       <c r="A2" s="16" t="s">
         <v>36</v>
       </c>
@@ -2513,7 +2645,7 @@
       </c>
       <c r="E2" s="18"/>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="60">
       <c r="A3" s="16" t="s">
         <v>38</v>
       </c>
@@ -2526,7 +2658,7 @@
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
     </row>
-    <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="180">
       <c r="A4" s="16" t="s">
         <v>40</v>
       </c>
@@ -2539,7 +2671,7 @@
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
     </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="75">
       <c r="A5" s="19" t="s">
         <v>55</v>
       </c>
@@ -2552,7 +2684,7 @@
       <c r="D5" s="12"/>
       <c r="E5" s="20"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45">
       <c r="A6" s="16" t="s">
         <v>52</v>
       </c>
@@ -2563,7 +2695,7 @@
       <c r="D6" s="17"/>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="45">
       <c r="A7" s="16" t="s">
         <v>57</v>
       </c>
@@ -2576,7 +2708,7 @@
       <c r="D7" s="17"/>
       <c r="E7" s="18"/>
     </row>
-    <row r="8" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="195">
       <c r="A8" s="16" t="s">
         <v>61</v>
       </c>
@@ -2589,7 +2721,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18"/>
     </row>
-    <row r="9" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="105">
       <c r="A9" s="16" t="s">
         <v>64</v>
       </c>
@@ -2602,7 +2734,7 @@
       <c r="D9" s="17"/>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="210">
       <c r="A10" s="16" t="s">
         <v>68</v>
       </c>
@@ -2617,7 +2749,7 @@
       </c>
       <c r="E10" s="18"/>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="60">
       <c r="A11" s="16" t="s">
         <v>72</v>
       </c>
@@ -2628,7 +2760,7 @@
       <c r="D11" s="17"/>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="210">
       <c r="A12" s="16" t="s">
         <v>77</v>
       </c>
@@ -2643,7 +2775,7 @@
       </c>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="105">
       <c r="A13" s="16" t="s">
         <v>78</v>
       </c>
@@ -2658,7 +2790,7 @@
       </c>
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="45">
       <c r="A14" s="16" t="s">
         <v>82</v>
       </c>
@@ -2671,7 +2803,7 @@
       <c r="D14" s="17"/>
       <c r="E14" s="18"/>
     </row>
-    <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="165">
       <c r="A15" s="16" t="s">
         <v>85</v>
       </c>
@@ -2686,7 +2818,7 @@
       </c>
       <c r="E15" s="18"/>
     </row>
-    <row r="16" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="270">
       <c r="A16" s="16" t="s">
         <v>89</v>
       </c>
@@ -2701,7 +2833,7 @@
       </c>
       <c r="E16" s="18"/>
     </row>
-    <row r="17" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="180">
       <c r="A17" s="16" t="s">
         <v>95</v>
       </c>
@@ -2714,46 +2846,115 @@
       <c r="D17" s="17"/>
       <c r="E17" s="18"/>
     </row>
-    <row r="18" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="180">
       <c r="A18" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>98</v>
       </c>
       <c r="C18" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="1:5" ht="105">
+      <c r="A19" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="18"/>
-    </row>
-    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="B19" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="C19" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>103</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="18"/>
     </row>
-    <row r="20" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="195">
       <c r="A20" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>105</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>106</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>107</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="1:5" ht="225">
+      <c r="A21" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" spans="1:5" ht="75">
+      <c r="A22" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" ht="270">
+      <c r="A23" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" spans="1:5" ht="195">
+      <c r="A24" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="1:5" ht="105">
+      <c r="A25" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>